<commit_message>
adding another graphic in the last screen
</commit_message>
<xml_diff>
--- a/inputTest.xlsx
+++ b/inputTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooper\Desktop\IC_Kevin\Estudando_Dados\repositas\Scientific-Initiation\webVersio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDF1D5F-2765-4648-B144-CA7CD2748DB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8326932B-21CB-49E2-81A6-1FF44C93CA68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{0B83699C-DFB6-49D9-A632-7785FB4DD04A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>availabilityLoss</t>
   </si>
@@ -61,18 +61,6 @@
   </si>
   <si>
     <t>costMaintainingInput</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -436,7 +424,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,158 +481,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>20</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
     </row>

</xml_diff>